<commit_message>
commit from mac 2016/09/09
</commit_message>
<xml_diff>
--- a/魅族移动端等级认证/王江川移动端开发序列初始化职级申请.xlsx
+++ b/魅族移动端等级认证/王江川移动端开发序列初始化职级申请.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuicui/Desktop/魅族移动端等级认证/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cuicui/Documents/MeiZu/魅族移动端等级认证/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="申请表" sheetId="1" r:id="rId1"/>
@@ -1089,62 +1089,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开发和维护的公共控件的信息：http://review.rnd.meizu.com/l/#/q/wangjiangchuan  
-(有一些由于迟迟没开通代码提交权限，挂在其他人名下)</t>
-    <rPh sb="0" eb="1">
-      <t>kai'fa</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>he</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>wei'hu</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>de</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>gon'gong</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>kong'jian</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>de</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>xin'xi</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>you'yi'xie</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>you'yu</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>chi'chi</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>mei'kai'tong</t>
-    </rPh>
-    <rPh sb="76" eb="77">
-      <t>dai'ma</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ti'jiao'quan'xian</t>
-    </rPh>
-    <rPh sb="83" eb="84">
-      <t>gua'zai</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>qi'ta'ren</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>ming'xia</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>查找相似图片类库开发：http://redmine.meizu.com/documents/1935</t>
     <rPh sb="0" eb="1">
       <t>cha'zhao'xiang'si'tu'pian</t>
@@ -1155,11 +1099,6 @@
     <rPh sb="8" eb="9">
       <t>kai'fa</t>
     </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Android系统动画作用介绍： http://redmine.meizu.com/documents/2455
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1387,6 +1326,76 @@
   </si>
   <si>
     <t>Flyme</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开发和维护的公共控件的信息：http://review.rnd.meizu.com/l/#/q/wangjiangchuan  
+(有一些由于迟迟没开通代码提交权限，组内成员帮忙提交的代码)</t>
+    <rPh sb="0" eb="1">
+      <t>kai'fa</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>he</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>wei'hu</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>de</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>gon'gong</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>kong'jian</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>de</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>xin'xi</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>you'yi'xie</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>you'yu</t>
+    </rPh>
+    <rPh sb="71" eb="72">
+      <t>chi'chi</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>mei'kai'tong</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>dai'ma</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ti'jiao'quan'xian</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>zu'nei</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>cheng'yuan</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>bang'm</t>
+    </rPh>
+    <rPh sb="89" eb="90">
+      <t>ti'jiao</t>
+    </rPh>
+    <rPh sb="91" eb="92">
+      <t>de</t>
+    </rPh>
+    <rPh sb="92" eb="93">
+      <t>dai'ma</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Android系统动画作用介绍： http://redmine.meizu.com/documents/2455
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1711,8 +1720,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1720,14 +1738,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1738,16 +1819,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1756,71 +1831,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1832,12 +1847,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2125,7 +2134,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B36" sqref="B36:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2142,28 +2151,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="A1" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -2175,35 +2184,35 @@
       <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="64">
+      <c r="D3" s="38">
         <v>502332</v>
       </c>
-      <c r="E3" s="49"/>
+      <c r="E3" s="39"/>
       <c r="F3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="H3" s="46"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="48"/>
+      <c r="D4" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="37"/>
     </row>
     <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
@@ -2215,29 +2224,29 @@
       <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="53"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="H5" s="48"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -2247,10 +2256,10 @@
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="48"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="14" t="s">
         <v>11</v>
       </c>
@@ -2262,194 +2271,194 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
     </row>
     <row r="9" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
     </row>
     <row r="11" spans="1:8" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="25" t="s">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="58" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="22" t="s">
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
     </row>
     <row r="15" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="57" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="22" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="57" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="22" t="s">
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
     </row>
     <row r="17" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="57" t="s">
-        <v>143</v>
-      </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="22" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="24"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="57" t="s">
+      <c r="B18" s="22"/>
+      <c r="C18" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="22" t="s">
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27"/>
     </row>
     <row r="20" spans="1:8" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
     </row>
     <row r="21" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -2458,14 +2467,14 @@
       <c r="B22" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
     </row>
     <row r="23" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
@@ -2474,14 +2483,14 @@
       <c r="B23" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
     </row>
     <row r="24" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -2490,50 +2499,50 @@
       <c r="B24" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
     </row>
     <row r="26" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="25" t="s">
+      <c r="B26" s="47"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="33"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
     </row>
     <row r="28" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
@@ -2547,197 +2556,165 @@
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="1:8" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
     </row>
     <row r="30" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25" t="s">
+      <c r="B30" s="47"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="33"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
     </row>
     <row r="31" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39" t="s">
+      <c r="A32" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
     </row>
     <row r="34" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21">
         <v>1</v>
       </c>
-      <c r="B35" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
+      <c r="B35" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
     </row>
     <row r="36" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>2</v>
       </c>
-      <c r="B36" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="38"/>
+      <c r="B36" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
     </row>
     <row r="37" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="8">
         <v>3</v>
       </c>
-      <c r="B37" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
+      <c r="B37" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
     </row>
     <row r="38" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>4</v>
       </c>
-      <c r="B38" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
+      <c r="B38" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
     </row>
     <row r="39" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>5</v>
       </c>
-      <c r="B39" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
+      <c r="B39" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F16:H16"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="A8:H8"/>
@@ -2754,13 +2731,45 @@
     <mergeCell ref="B36:H36"/>
     <mergeCell ref="B37:H37"/>
     <mergeCell ref="B38:H38"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="7">
@@ -2812,23 +2821,23 @@
       <c r="B1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62" t="s">
+      <c r="E1" s="64"/>
+      <c r="F1" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="62"/>
+      <c r="G1" s="64"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="60" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="61" t="s">
         <v>107</v>
       </c>
       <c r="E2" s="11" t="s">
@@ -2838,11 +2847,11 @@
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="63"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="11" t="s">
         <v>82</v>
       </c>
@@ -2850,11 +2859,11 @@
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="63"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="11" t="s">
         <v>81</v>
       </c>
@@ -2862,13 +2871,13 @@
       <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="60" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="60"/>
+      <c r="D5" s="62"/>
       <c r="E5" s="11" t="s">
         <v>84</v>
       </c>
@@ -2876,11 +2885,11 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="63"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="60"/>
+      <c r="D6" s="62"/>
       <c r="E6" s="11" t="s">
         <v>80</v>
       </c>
@@ -2888,11 +2897,11 @@
       <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="63"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="60"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="11" t="s">
         <v>79</v>
       </c>
@@ -2900,17 +2909,17 @@
       <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="60" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="61" t="s">
         <v>108</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -2918,169 +2927,169 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="60"/>
+      <c r="D9" s="62"/>
       <c r="E9" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="60"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="60"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F10" s="60"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="60"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="60"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="60"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="60"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="60"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="11" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="60"/>
+      <c r="D14" s="62"/>
       <c r="E14" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="60"/>
+      <c r="F14" s="62"/>
       <c r="G14" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="60"/>
+      <c r="D15" s="62"/>
       <c r="E15" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="60"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="60" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="61"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="60"/>
+      <c r="F16" s="62"/>
       <c r="G16" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="10" t="s">
         <v>53</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="F17" s="61"/>
+      <c r="F17" s="63"/>
       <c r="G17" s="11" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="60" t="s">
         <v>60</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -3088,13 +3097,13 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="28" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="60" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -3102,31 +3111,31 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="63"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="63"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="63"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="60" t="s">
         <v>69</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -3134,19 +3143,19 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="63"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="63"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="63" t="s">
+      <c r="A34" s="60" t="s">
         <v>73</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -3154,25 +3163,25 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="28" x14ac:dyDescent="0.2">
-      <c r="A35" s="63"/>
+      <c r="A35" s="60"/>
       <c r="B35" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="63"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="63"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="63"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="11" t="s">
         <v>78</v>
       </c>
@@ -3187,6 +3196,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D2:D16"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F8:F17"/>
+    <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A38"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
@@ -3194,11 +3208,6 @@
     <mergeCell ref="A16:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A30"/>
-    <mergeCell ref="D2:D16"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F8:F17"/>
-    <mergeCell ref="A31:A33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>